<commit_message>
photo sessions for new sodas dataset completed
</commit_message>
<xml_diff>
--- a/sodas_dataset_raw/session classes.xlsx
+++ b/sodas_dataset_raw/session classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\Image_processing_and_Dataset\sodas_dataset_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEA12D9-C529-4999-887C-8D5F50D6A7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407BFE52-0333-4D83-AAB0-F67E2CCA482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="21">
   <si>
     <t>Session number</t>
   </si>
@@ -69,15 +69,6 @@
     <t>coca cola lata 355 ml</t>
   </si>
   <si>
-    <t>out 2</t>
-  </si>
-  <si>
-    <t>out 1</t>
-  </si>
-  <si>
-    <t>out 3</t>
-  </si>
-  <si>
     <t>delaware punch lata 355 ml</t>
   </si>
   <si>
@@ -96,19 +87,7 @@
     <t>power ade mora azul botella de plastico 500 ml</t>
   </si>
   <si>
-    <t>out 4</t>
-  </si>
-  <si>
     <t>vacio</t>
-  </si>
-  <si>
-    <t>out 6</t>
-  </si>
-  <si>
-    <t>out 7</t>
-  </si>
-  <si>
-    <t>-----</t>
   </si>
 </sst>
 </file>
@@ -158,13 +137,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -447,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,7 +445,7 @@
     <col min="15" max="15" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,26 +473,8 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -524,16 +482,16 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>10</v>
@@ -547,46 +505,28 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
@@ -595,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -603,28 +543,28 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -632,28 +572,28 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -667,22 +607,22 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -696,22 +636,22 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -719,28 +659,28 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -748,19 +688,19 @@
         <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>10</v>
@@ -769,7 +709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -777,71 +717,71 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
@@ -850,18 +790,18 @@
         <v>9</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
@@ -870,58 +810,250 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
attempt to improve fridge detection
</commit_message>
<xml_diff>
--- a/sodas_dataset_raw/session classes.xlsx
+++ b/sodas_dataset_raw/session classes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Documents\Image_processing_and_Dataset\sodas_dataset_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407BFE52-0333-4D83-AAB0-F67E2CCA482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A3B014-355F-4B65-A1CB-B454B47BE3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>